<commit_message>
master branch first commit
</commit_message>
<xml_diff>
--- a/src/assets/document/Student_Template1.xlsx
+++ b/src/assets/document/Student_Template1.xlsx
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="1196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2153" uniqueCount="1195">
   <si>
     <t>Qualification</t>
   </si>
@@ -3712,9 +3712,6 @@
   </si>
   <si>
     <t>Address_Line_1</t>
-  </si>
-  <si>
-    <t>kabfv</t>
   </si>
   <si>
     <t>df</t>
@@ -4346,7 +4343,7 @@
   <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4437,17 +4434,13 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>1234</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11" t="s">
         <v>1193</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>1194</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>1195</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="8" t="s">

</xml_diff>